<commit_message>
Changing structure and theming. Still in progress.
</commit_message>
<xml_diff>
--- a/data/LocationData.xlsx
+++ b/data/LocationData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stichtingfontys-my.sharepoint.com/personal/412657_student_fontys_nl/Documents/_Fontys/TW4/Project Stage/FinalVersionSchedule/VesselScheduleProblem/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\GitLab\examples\application-examples\vessel_scheduling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_FFC65FC097D169D86E170BE0B37802867CCE0F42" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{705FF79B-17D2-40DC-AD9B-A838C20C1548}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6432889-D1F9-4ACA-BF85-D694822B075E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LocationData" sheetId="2" r:id="rId1"/>
@@ -23,9 +23,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="188">
   <si>
-    <t>i_Loc</t>
-  </si>
-  <si>
     <t>Latitude</t>
   </si>
   <si>
@@ -585,6 +582,9 @@
   </si>
   <si>
     <t>Unloading</t>
+  </si>
+  <si>
+    <t>i_loc</t>
   </si>
 </sst>
 </file>
@@ -624,7 +624,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -639,14 +639,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -684,9 +680,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -719,26 +715,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -771,26 +750,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -966,33 +928,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0741A27-0D33-4750-8DE9-76F34737FB41}">
   <dimension ref="A1:D176"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
       </c>
       <c r="B2">
         <v>22.488900000000001</v>
@@ -1004,9 +964,9 @@
         <v>738</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>-8.0555555559999998</v>
@@ -1018,9 +978,9 @@
         <v>577</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>-3.5336110000000001</v>
@@ -1032,9 +992,9 @@
         <v>258</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>-2.5649999999999999</v>
@@ -1046,9 +1006,9 @@
         <v>411</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>-20.7884999999999</v>
@@ -1060,9 +1020,9 @@
         <v>719</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>11.069476</v>
@@ -1074,9 +1034,9 @@
         <v>608</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>4.7387639999999998</v>
@@ -1088,9 +1048,9 @@
         <v>283</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>5.2892400000000004</v>
@@ -1102,9 +1062,9 @@
         <v>489</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>18.419934999999899</v>
@@ -1116,9 +1076,9 @@
         <v>601</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>13.921932</v>
@@ -1130,9 +1090,9 @@
         <v>415</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>18.949947099999999</v>
@@ -1144,9 +1104,9 @@
         <v>316</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>15.413885000000001</v>
@@ -1158,9 +1118,9 @@
         <v>299</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>8.5631989999999991</v>
@@ -1172,9 +1132,9 @@
         <v>434</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15">
         <v>-3.292189</v>
@@ -1186,9 +1146,9 @@
         <v>488</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>24.774781000000001</v>
@@ -1200,9 +1160,9 @@
         <v>661</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <v>-6.7410550000000002</v>
@@ -1214,9 +1174,9 @@
         <v>575</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <v>-15.258332999999899</v>
@@ -1228,9 +1188,9 @@
         <v>418</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19">
         <v>6.0935870000000003</v>
@@ -1242,9 +1202,9 @@
         <v>712</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <v>-4.7888380000000002</v>
@@ -1256,9 +1216,9 @@
         <v>552</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21">
         <v>-33.806725</v>
@@ -1270,9 +1230,9 @@
         <v>261</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22">
         <v>46.649510999999897</v>
@@ -1284,9 +1244,9 @@
         <v>603</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23">
         <v>46.329355999999898</v>
@@ -1298,9 +1258,9 @@
         <v>385</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24">
         <v>10.5389839999999</v>
@@ -1312,9 +1272,9 @@
         <v>321</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25">
         <v>10.028922999999899</v>
@@ -1326,9 +1286,9 @@
         <v>698</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26">
         <v>19.1169499999999</v>
@@ -1340,9 +1300,9 @@
         <v>354</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27">
         <v>17.970659999999999</v>
@@ -1354,9 +1314,9 @@
         <v>489</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28">
         <v>22.392150000000001</v>
@@ -1368,9 +1328,9 @@
         <v>361</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29">
         <v>19.1809499999999</v>
@@ -1382,9 +1342,9 @@
         <v>266</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30">
         <v>13.5927799999999</v>
@@ -1396,9 +1356,9 @@
         <v>272</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31">
         <v>15.7277799999999</v>
@@ -1410,9 +1370,9 @@
         <v>629</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32">
         <v>15.59981</v>
@@ -1424,9 +1384,9 @@
         <v>601</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33">
         <v>15.825620000000001</v>
@@ -1438,9 +1398,9 @@
         <v>499</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34">
         <v>12.4825</v>
@@ -1452,9 +1412,9 @@
         <v>525</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35">
         <v>9.9331899999999997</v>
@@ -1466,9 +1426,9 @@
         <v>296</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36">
         <v>9.99073999999999</v>
@@ -1480,9 +1440,9 @@
         <v>706</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37">
         <v>-4.5772199999999996</v>
@@ -1494,9 +1454,9 @@
         <v>482</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38">
         <v>-5.0891699999999904</v>
@@ -1508,9 +1468,9 @@
         <v>736</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B39">
         <v>9.3522199999999902</v>
@@ -1522,9 +1482,9 @@
         <v>663</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40">
         <v>9.3545099999999994</v>
@@ -1536,9 +1496,9 @@
         <v>663</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41">
         <v>-2.1961599999999999</v>
@@ -1550,9 +1510,9 @@
         <v>366</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42">
         <v>8.9481399999999898</v>
@@ -1564,9 +1524,9 @@
         <v>701</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43">
         <v>26.5333299999999</v>
@@ -1578,9 +1538,9 @@
         <v>512</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44">
         <v>-12.05659</v>
@@ -1592,9 +1552,9 @@
         <v>466</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45">
         <v>3.8801000000000001</v>
@@ -1606,9 +1566,9 @@
         <v>398</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B46">
         <v>17.937379999999902</v>
@@ -1620,9 +1580,9 @@
         <v>739</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B47">
         <v>10.39972</v>
@@ -1634,9 +1594,9 @@
         <v>404</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B48">
         <v>10.9685399999999</v>
@@ -1648,9 +1608,9 @@
         <v>530</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B49">
         <v>11.240789999999899</v>
@@ -1662,9 +1622,9 @@
         <v>345</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B50">
         <v>18.543489999999899</v>
@@ -1676,9 +1636,9 @@
         <v>614</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B51">
         <v>-16.996389999999899</v>
@@ -1690,9 +1650,9 @@
         <v>255</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B52">
         <v>12.241070000000001</v>
@@ -1704,9 +1664,9 @@
         <v>542</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B53">
         <v>-33.036000000000001</v>
@@ -1718,9 +1678,9 @@
         <v>704</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B54">
         <v>-33.594729999999899</v>
@@ -1732,9 +1692,9 @@
         <v>567</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B55">
         <v>-27.088859999999901</v>
@@ -1746,9 +1706,9 @@
         <v>314</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B56">
         <v>-27.06812</v>
@@ -1760,9 +1720,9 @@
         <v>291</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B57">
         <v>-26.342979999999901</v>
@@ -1774,9 +1734,9 @@
         <v>694</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B58">
         <v>-38.719589999999997</v>
@@ -1788,9 +1748,9 @@
         <v>301</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B59">
         <v>-32.946820000000002</v>
@@ -1802,9 +1762,9 @@
         <v>642</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B60">
         <v>-38.554499999999898</v>
@@ -1816,9 +1776,9 @@
         <v>715</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B61">
         <v>-34.613149999999898</v>
@@ -1830,9 +1790,9 @@
         <v>743</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B62">
         <v>-34.92145</v>
@@ -1844,9 +1804,9 @@
         <v>545</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B63">
         <v>-34.903280000000002</v>
@@ -1858,9 +1818,9 @@
         <v>268</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B64">
         <v>-25.427779999999899</v>
@@ -1872,9 +1832,9 @@
         <v>485</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B65">
         <v>-28.466670000000001</v>
@@ -1886,9 +1846,9 @@
         <v>450</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B66">
         <v>-26.907779999999899</v>
@@ -1900,9 +1860,9 @@
         <v>630</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B67">
         <v>-26.11694</v>
@@ -1914,9 +1874,9 @@
         <v>742</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B68">
         <v>-25.5162599999999</v>
@@ -1928,9 +1888,9 @@
         <v>504</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B69">
         <v>-23.960829999999898</v>
@@ -1942,9 +1902,9 @@
         <v>736</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B70">
         <v>-22.979310000000002</v>
@@ -1956,9 +1916,9 @@
         <v>473</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B71">
         <v>-22.906420000000001</v>
@@ -1970,9 +1930,9 @@
         <v>417</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B72">
         <v>-22.906420000000001</v>
@@ -1984,9 +1944,9 @@
         <v>462</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B73">
         <v>-12.971109999999999</v>
@@ -1998,9 +1958,9 @@
         <v>295</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B74">
         <v>14.6937</v>
@@ -2012,9 +1972,9 @@
         <v>488</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B75">
         <v>20.941879999999902</v>
@@ -2026,9 +1986,9 @@
         <v>516</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B76">
         <v>13.452739999999899</v>
@@ -2040,9 +2000,9 @@
         <v>677</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B77">
         <v>10.65</v>
@@ -2054,9 +2014,9 @@
         <v>450</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B78">
         <v>9.5379500000000004</v>
@@ -2068,9 +2028,9 @@
         <v>745</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B79">
         <v>8.4871400000000001</v>
@@ -2082,9 +2042,9 @@
         <v>326</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B80">
         <v>6.3005399999999998</v>
@@ -2096,9 +2056,9 @@
         <v>356</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B81">
         <v>5.8769299999999998</v>
@@ -2110,9 +2070,9 @@
         <v>293</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B82">
         <v>30.420179999999899</v>
@@ -2124,9 +2084,9 @@
         <v>532</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B83">
         <v>35.767270000000003</v>
@@ -2138,9 +2098,9 @@
         <v>517</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B84">
         <v>4.8981599999999998</v>
@@ -2152,9 +2112,9 @@
         <v>319</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B85">
         <v>5.6698000000000004</v>
@@ -2166,9 +2126,9 @@
         <v>739</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B86">
         <v>6.1287399999999996</v>
@@ -2180,9 +2140,9 @@
         <v>436</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B87">
         <v>36.510759999999912</v>
@@ -2194,9 +2154,9 @@
         <v>508</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B88">
         <v>6.3653599999999999</v>
@@ -2208,9 +2168,9 @@
         <v>655</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B89">
         <v>36.732250000000001</v>
@@ -2222,9 +2182,9 @@
         <v>731</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B90">
         <v>6.4540699999999998</v>
@@ -2236,9 +2196,9 @@
         <v>747</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B91">
         <v>0.29122999999999999</v>
@@ -2250,9 +2210,9 @@
         <v>288</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B92">
         <v>4.0482699999999996</v>
@@ -2264,9 +2224,9 @@
         <v>440</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B93">
         <v>2.9372500000000001</v>
@@ -2278,9 +2238,9 @@
         <v>334</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B94">
         <v>36.769459999999903</v>
@@ -2292,9 +2252,9 @@
         <v>587</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B95">
         <v>-8.8368199999999906</v>
@@ -2306,9 +2266,9 @@
         <v>513</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B96">
         <v>45.326729999999898</v>
@@ -2320,9 +2280,9 @@
         <v>291</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B97">
         <v>-22.9575</v>
@@ -2334,9 +2294,9 @@
         <v>560</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B98">
         <v>43.056109999999897</v>
@@ -2348,9 +2308,9 @@
         <v>312</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B99">
         <v>-33.011670000000002</v>
@@ -2362,9 +2322,9 @@
         <v>300</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B100">
         <v>-33.925840000000001</v>
@@ -2376,9 +2336,9 @@
         <v>344</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B101">
         <v>41.323549999999898</v>
@@ -2390,9 +2350,9 @@
         <v>416</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B102">
         <v>32.11486</v>
@@ -2404,9 +2364,9 @@
         <v>349</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B103">
         <v>40.98272</v>
@@ -2418,9 +2378,9 @@
         <v>591</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B104">
         <v>31.201759999999901</v>
@@ -2432,9 +2392,9 @@
         <v>354</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B105">
         <v>46.299140000000001</v>
@@ -2446,9 +2406,9 @@
         <v>269</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B106">
         <v>46.485720000000001</v>
@@ -2460,9 +2420,9 @@
         <v>268</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B107">
         <v>-29.857900000000001</v>
@@ -2474,9 +2434,9 @@
         <v>316</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B108">
         <v>46.965910000000001</v>
@@ -2488,9 +2448,9 @@
         <v>718</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B109">
         <v>-28.783009999999901</v>
@@ -2502,9 +2462,9 @@
         <v>251</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B110">
         <v>31.2653099999999</v>
@@ -2516,9 +2476,9 @@
         <v>252</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B111">
         <v>-25.962219999999999</v>
@@ -2530,9 +2490,9 @@
         <v>312</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B112">
         <v>-25.965529999999902</v>
@@ -2544,9 +2504,9 @@
         <v>652</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B113">
         <v>68.979169999999897</v>
@@ -2558,9 +2518,9 @@
         <v>586</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B114">
         <v>36.811959999999907</v>
@@ -2572,9 +2532,9 @@
         <v>749</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B115">
         <v>-19.843610000000002</v>
@@ -2586,9 +2546,9 @@
         <v>452</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B116">
         <v>29.526669999999999</v>
@@ -2600,9 +2560,9 @@
         <v>740</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B117">
         <v>33.893320000000003</v>
@@ -2614,9 +2574,9 @@
         <v>482</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B118">
         <v>34.433520000000001</v>
@@ -2628,9 +2588,9 @@
         <v>584</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B119">
         <v>34.507800000000003</v>
@@ -2642,9 +2602,9 @@
         <v>532</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B120">
         <v>55.81353</v>
@@ -2656,9 +2616,9 @@
         <v>413</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B121">
         <v>44.72439</v>
@@ -2670,9 +2630,9 @@
         <v>457</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B122">
         <v>-6.8234899999999996</v>
@@ -2684,9 +2644,9 @@
         <v>696</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B123">
         <v>-4.0546600000000002</v>
@@ -2698,9 +2658,9 @@
         <v>424</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B124">
         <v>47.231349999999892</v>
@@ -2712,9 +2672,9 @@
         <v>532</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B125">
         <v>41.64228</v>
@@ -2726,9 +2686,9 @@
         <v>510</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B126">
         <v>42.142719999999997</v>
@@ -2740,9 +2700,9 @@
         <v>601</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B127">
         <v>-0.35816999999999999</v>
@@ -2754,9 +2714,9 @@
         <v>619</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B128">
         <v>11.58901</v>
@@ -2768,9 +2728,9 @@
         <v>470</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B129">
         <v>-11.702159999999999</v>
@@ -2782,9 +2742,9 @@
         <v>497</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B130">
         <v>-12.16672</v>
@@ -2796,9 +2756,9 @@
         <v>540</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B131">
         <v>10.4395899999999</v>
@@ -2810,9 +2770,9 @@
         <v>642</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B132">
         <v>2.0371100000000002</v>
@@ -2824,9 +2784,9 @@
         <v>499</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B133">
         <v>-18.1492</v>
@@ -2838,9 +2798,9 @@
         <v>625</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B134">
         <v>-4.6200099999999997</v>
@@ -2852,9 +2812,9 @@
         <v>552</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B135">
         <v>-4.6200099999999997</v>
@@ -2866,9 +2826,9 @@
         <v>411</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B136">
         <v>-20.161939999999898</v>
@@ -2880,9 +2840,9 @@
         <v>456</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B137">
         <v>24.860800000000001</v>
@@ -2894,9 +2854,9 @@
         <v>537</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B138">
         <v>23.0333299999999</v>
@@ -2908,9 +2868,9 @@
         <v>649</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B139">
         <v>19.07283</v>
@@ -2922,9 +2882,9 @@
         <v>720</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B140">
         <v>4.1752099999999999</v>
@@ -2936,9 +2896,9 @@
         <v>638</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B141">
         <v>12.91723</v>
@@ -2950,9 +2910,9 @@
         <v>509</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B142">
         <v>11.24802</v>
@@ -2964,9 +2924,9 @@
         <v>340</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B143">
         <v>9.9398800000000005</v>
@@ -2978,9 +2938,9 @@
         <v>508</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B144">
         <v>8.8811300000000006</v>
@@ -2992,9 +2952,9 @@
         <v>322</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B145">
         <v>8.7673500000000004</v>
@@ -3006,9 +2966,9 @@
         <v>576</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B146">
         <v>6.9354800000000001</v>
@@ -3020,9 +2980,9 @@
         <v>734</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B147">
         <v>13.08784</v>
@@ -3034,9 +2994,9 @@
         <v>341</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B148">
         <v>13.24751</v>
@@ -3048,9 +3008,9 @@
         <v>491</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B149">
         <v>16.960360000000001</v>
@@ -3062,9 +3022,9 @@
         <v>743</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B150">
         <v>17.68009</v>
@@ -3076,9 +3036,9 @@
         <v>514</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B151">
         <v>20.316410000000001</v>
@@ -3090,9 +3050,9 @@
         <v>489</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B152">
         <v>22.562629999999899</v>
@@ -3104,9 +3064,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B153">
         <v>22.3384</v>
@@ -3118,9 +3078,9 @@
         <v>506</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B154">
         <v>16.80528</v>
@@ -3132,9 +3092,9 @@
         <v>654</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B155">
         <v>16.661100000000001</v>
@@ -3146,9 +3106,9 @@
         <v>256</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B156">
         <v>3.7755000000000001</v>
@@ -3160,9 +3120,9 @@
         <v>287</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B157">
         <v>-2.0301</v>
@@ -3174,9 +3134,9 @@
         <v>718</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B158">
         <v>10.60932</v>
@@ -3188,9 +3148,9 @@
         <v>453</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B159">
         <v>10.03711</v>
@@ -3202,9 +3162,9 @@
         <v>377</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B160">
         <v>10.82302</v>
@@ -3216,9 +3176,9 @@
         <v>330</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B161">
         <v>20.864809999999999</v>
@@ -3230,9 +3190,9 @@
         <v>738</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B162">
         <v>16.0677799999999</v>
@@ -3244,9 +3204,9 @@
         <v>658</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B163">
         <v>13.7764799999999</v>
@@ -3258,9 +3218,9 @@
         <v>611</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B164">
         <v>-3.3198699999999999</v>
@@ -3272,9 +3232,9 @@
         <v>636</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B165">
         <v>-1.26753</v>
@@ -3286,9 +3246,9 @@
         <v>670</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B166">
         <v>-5.1486099999999997</v>
@@ -3300,9 +3260,9 @@
         <v>746</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B167">
         <v>14.604200000000001</v>
@@ -3314,9 +3274,9 @@
         <v>510</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B168">
         <v>6.9102800000000002</v>
@@ -3328,9 +3288,9 @@
         <v>534</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B169">
         <v>8.1480999999999906</v>
@@ -3342,9 +3302,9 @@
         <v>607</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B170">
         <v>10.31672</v>
@@ -3356,9 +3316,9 @@
         <v>607</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B171">
         <v>8.2288999999999906</v>
@@ -3370,9 +3330,9 @@
         <v>612</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B172">
         <v>8.4822199999999999</v>
@@ -3384,9 +3344,9 @@
         <v>418</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B173">
         <v>8.9472199999999997</v>
@@ -3398,9 +3358,9 @@
         <v>318</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B174">
         <v>9.7889999999999997</v>
@@ -3412,9 +3372,9 @@
         <v>587</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B175">
         <v>7.0730599999999999</v>
@@ -3426,9 +3386,9 @@
         <v>320</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B176">
         <v>-9.4772300000000005</v>
@@ -3449,45 +3409,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F92C99D-2C90-49DD-AE6C-C35372F95EE4}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" t="s">
         <v>179</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>180</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>181</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>183</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3496,9 +3456,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3507,9 +3467,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B6">
         <v>1</v>

</xml_diff>